<commit_message>
End prop ver 1.1
</commit_message>
<xml_diff>
--- a/Актуализация групп.xlsx
+++ b/Актуализация групп.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>TCS</t>
   </si>
@@ -27,6 +27,9 @@
     <t>Polynom</t>
   </si>
   <si>
+    <t>Выбор группы Polynom</t>
+  </si>
+  <si>
     <t>Химикотермическая обработка (металлургическая)</t>
   </si>
   <si>
@@ -72,12 +75,20 @@
     <t>Разделительные</t>
   </si>
   <si>
+    <t>0 - Справочник технолога//Операции/Обработка давлением/Разделительные/</t>
+  </si>
+  <si>
     <t>Деревообработка</t>
   </si>
   <si>
     <t>Электромонтаж</t>
   </si>
   <si>
+    <t>0 - Справочник технолога//Операции/Электромонтаж/
+1 - Справочник технолога//Операции/Электромонтаж/Электромонтаж/
+2 - Справочник технолога//Операции/Электромонтаж/Электромонтаж/Электромонтаж/</t>
+  </si>
+  <si>
     <t>Резка (металлургическая)</t>
   </si>
   <si>
@@ -90,6 +101,11 @@
     <t>Сборка</t>
   </si>
   <si>
+    <t>0 - Справочник технолога//Операции/Сборка/
+1 - Справочник технолога//Операции/Сборка/Сборка/
+2 - Справочник технолога//Операции/Сборка/Сборка/Сборка/</t>
+  </si>
+  <si>
     <t>Очистка (металлургическая)</t>
   </si>
   <si>
@@ -105,6 +121,10 @@
     <t>Испытания</t>
   </si>
   <si>
+    <t>0 - Справочник технолога//Операции/Испытания/
+1 - Справочник технолога//Операции/Испытания/Прочие операции/Испытания/</t>
+  </si>
+  <si>
     <t>Обслуживание шасси</t>
   </si>
   <si>
@@ -114,9 +134,15 @@
     <t>Вулканизация</t>
   </si>
   <si>
+    <t>0 - Справочник технолога//Операции/Формообразование из полимерных материалов, керамик/Формообразование из полимерных материалов, керамики, стекла и резины/Вулканизация/</t>
+  </si>
+  <si>
     <t>Прессование</t>
   </si>
   <si>
+    <t>0 - Справочник технолога//Операции/Формообразование из полимерных материалов, керамик/Формообразование из полимерных материалов, керамики, стекла и резины/Прессование/</t>
+  </si>
+  <si>
     <t>Зубообрабатывающие</t>
   </si>
   <si>
@@ -129,12 +155,20 @@
     <t>Маркирование</t>
   </si>
   <si>
+    <t>0 - Справочник технолога//Операции/Операции общего назначения/Маркирование/
+1 - Справочник технолога//Операции/Операции общего назначения/Маркирование/Маркирование/</t>
+  </si>
+  <si>
     <t>Программные</t>
   </si>
   <si>
     <t>Консервация</t>
   </si>
   <si>
+    <t>0 - Справочник технолога//Операции/Консервация и упаковывание/Консервация/
+1 - Справочник технолога//Операции/Консервация и упаковывание/Консервация/Консервация/</t>
+  </si>
+  <si>
     <t>Лакокраска</t>
   </si>
   <si>
@@ -178,6 +212,10 @@
   </si>
   <si>
     <t>Сварка</t>
+  </si>
+  <si>
+    <t>0 - Справочник технолога//Операции/Сварка/
+1 - Справочник технолога//Операции/Сварка/Прочие операции/Сварка/</t>
   </si>
   <si>
     <t>Правка (металлургическая)</t>
@@ -272,8 +310,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -576,403 +620,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="91.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="91.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>